<commit_message>
Updated Playoff Bracket, Box Scores
Data Input for 1st game
</commit_message>
<xml_diff>
--- a/2024/Playoffs/BoxScores.xlsx
+++ b/2024/Playoffs/BoxScores.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LunchProjects\GitHub\NHLStats\2024\Playoffs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\NHLStats\2024\Playoffs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C77A2EF-2F9F-43DB-B7F7-33C673364DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2880" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3027" uniqueCount="479">
   <si>
     <t>Boston Bruins</t>
   </si>
@@ -1477,12 +1478,30 @@
   </si>
   <si>
     <t>Lucas Johansen</t>
+  </si>
+  <si>
+    <t>FO%</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>SV</t>
+  </si>
+  <si>
+    <t>SV%</t>
+  </si>
+  <si>
+    <t>SOSA</t>
+  </si>
+  <si>
+    <t>SOS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -2043,7 +2062,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2183,16 +2202,16 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" location="'Scores (4-20-24)'!A1" display="Scores"/>
-    <hyperlink ref="B3" location="'Scores (4-21-24)'!A1" display="Scores"/>
-    <hyperlink ref="B4" location="'Scores (4-22-24)'!A1" display="Scores"/>
-    <hyperlink ref="B5" location="'Scores (4-23-24)'!A1" display="Scores"/>
-    <hyperlink ref="B6" location="'Scores (4-24-24)'!A1" display="Scores"/>
-    <hyperlink ref="B7" location="'Scores (4-25-24)'!A1" display="Scores"/>
-    <hyperlink ref="B8" location="'Scores (4-26-24)'!A1" display="Scores"/>
-    <hyperlink ref="B9" location="'Scores (4-27-24)'!A1" display="Scores"/>
-    <hyperlink ref="B10" location="'Scores (4-28-24)'!A1" display="Scores"/>
-    <hyperlink ref="B11" location="'Scores (4-29-24)'!A1" display="Scores"/>
+    <hyperlink ref="B2" location="'Scores (4-20-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" location="'Scores (4-21-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" location="'Scores (4-22-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" location="'Scores (4-23-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" location="'Scores (4-24-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" location="'Scores (4-25-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" location="'Scores (4-26-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" location="'Scores (4-27-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" location="'Scores (4-28-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" location="'Scores (4-29-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2200,7 +2219,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2302,21 +2321,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A7" location="'Offense (4-26-24)'!A1" display="Offense"/>
-    <hyperlink ref="A8" location="'Goalies (4-26-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="A7" location="'Offense (4-26-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="A8" location="'Goalies (4-26-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -2329,7 +2348,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2431,21 +2450,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A7" location="'Offense (4-27-24)'!A1" display="Offense"/>
-    <hyperlink ref="A8" location="'Goalies (4-27-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="A7" location="'Offense (4-27-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="A8" location="'Goalies (4-27-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -2458,7 +2477,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2560,21 +2579,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A7" location="'Offense (4-28-24)'!A1" display="Offense"/>
-    <hyperlink ref="A8" location="'Goalies (4-28-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="A7" location="'Offense (4-28-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="A8" location="'Goalies (4-28-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -2587,7 +2606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2669,21 +2688,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A5" location="'Offense (4-29-24)'!A1" display="Offense"/>
-    <hyperlink ref="A6" location="'Goalies (4-29-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="A5" location="'Offense (4-29-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
+    <hyperlink ref="A6" location="'Goalies (4-29-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -2696,7 +2715,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:U73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7243,19 +7262,19 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:U187">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U187">
     <sortCondition ref="C2:C187"/>
     <sortCondition ref="A2:A187"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-20-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (4-20-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7464,18 +7483,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L5">
     <sortCondition ref="C2:C5"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-20-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-20-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:T145"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16482,7 +16501,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:X204">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X204">
     <sortCondition ref="C2:C204"/>
     <sortCondition ref="A2:A204"/>
   </sortState>
@@ -16491,7 +16510,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16852,18 +16871,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L9">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L9">
     <sortCondition ref="C2:C9"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-21-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-21-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:U145"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -25873,12 +25892,12 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:X263">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X263">
     <sortCondition ref="C2:C263"/>
     <sortCondition ref="A2:A263"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-22-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (4-22-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25886,7 +25905,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26247,18 +26266,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:N9">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N9">
     <sortCondition ref="C2:C9"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-22-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-22-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26474,7 +26493,7 @@
       <c r="M55" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="B2:B9">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B9">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26482,7 +26501,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:U145"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -35492,12 +35511,12 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:X263">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X263">
     <sortCondition ref="C2:C263"/>
     <sortCondition ref="A2:A263"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-23-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (4-23-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -35505,7 +35524,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -35866,40 +35885,2564 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:N9">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N9">
     <sortCondition ref="C2:C9"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-23-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-23-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="23" width="9.140625" style="1"/>
+    <col min="24" max="24" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>10</v>
+      </c>
+      <c r="P2" s="18">
+        <v>0.41249999999999998</v>
+      </c>
+      <c r="Q2" s="18">
+        <v>0</v>
+      </c>
+      <c r="R2" s="18">
+        <v>2.2916666666666665E-2</v>
+      </c>
+      <c r="S2" s="18">
+        <v>0.38958333333333334</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>17</v>
+      </c>
+      <c r="P3" s="18">
+        <v>0.50972222222222219</v>
+      </c>
+      <c r="Q3" s="18">
+        <v>0.13958333333333334</v>
+      </c>
+      <c r="R3" s="18">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S3" s="18">
+        <v>0.30763888888888891</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2</v>
+      </c>
+      <c r="M4" s="1">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>18</v>
+      </c>
+      <c r="P4" s="18">
+        <v>0.53541666666666665</v>
+      </c>
+      <c r="Q4" s="18">
+        <v>0.12430555555555556</v>
+      </c>
+      <c r="R4" s="18">
+        <v>8.5416666666666669E-2</v>
+      </c>
+      <c r="S4" s="18">
+        <v>0.32569444444444445</v>
+      </c>
+      <c r="T4" s="1">
+        <v>8</v>
+      </c>
+      <c r="U4" s="1">
+        <v>7</v>
+      </c>
+      <c r="V4" s="1">
+        <v>53.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>4</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>12</v>
+      </c>
+      <c r="P5" s="18">
+        <v>0.40069444444444446</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>0</v>
+      </c>
+      <c r="R5" s="18">
+        <v>0</v>
+      </c>
+      <c r="S5" s="18">
+        <v>0.40069444444444446</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>12</v>
+      </c>
+      <c r="P6" s="18">
+        <v>0.28541666666666665</v>
+      </c>
+      <c r="Q6" s="18">
+        <v>0</v>
+      </c>
+      <c r="R6" s="18">
+        <v>5.8333333333333334E-2</v>
+      </c>
+      <c r="S6" s="18">
+        <v>0.22708333333333333</v>
+      </c>
+      <c r="T6" s="1">
+        <v>2</v>
+      </c>
+      <c r="U6" s="1">
+        <v>2</v>
+      </c>
+      <c r="V6" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1</v>
+      </c>
+      <c r="P7" s="18">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="Q7" s="18">
+        <v>0</v>
+      </c>
+      <c r="R7" s="18">
+        <v>0</v>
+      </c>
+      <c r="S7" s="18">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1</v>
+      </c>
+      <c r="O8" s="1">
+        <v>18</v>
+      </c>
+      <c r="P8" s="18">
+        <v>0.78263888888888888</v>
+      </c>
+      <c r="Q8" s="18">
+        <v>0.14930555555555555</v>
+      </c>
+      <c r="R8" s="18">
+        <v>0.10347222222222222</v>
+      </c>
+      <c r="S8" s="18">
+        <v>0.52986111111111112</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="1">
+        <v>0</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>2</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>10</v>
+      </c>
+      <c r="P9" s="18">
+        <v>0.37847222222222221</v>
+      </c>
+      <c r="Q9" s="18">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="R9" s="18">
+        <v>0</v>
+      </c>
+      <c r="S9" s="18">
+        <v>0.35972222222222222</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>14</v>
+      </c>
+      <c r="P10" s="18">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="Q10" s="18">
+        <v>0.12152777777777778</v>
+      </c>
+      <c r="R10" s="18">
+        <v>0</v>
+      </c>
+      <c r="S10" s="18">
+        <v>0.40625</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
+      <c r="U10" s="1">
+        <v>0</v>
+      </c>
+      <c r="V10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>3</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1">
+        <v>17</v>
+      </c>
+      <c r="P11" s="18">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="Q11" s="18">
+        <v>0</v>
+      </c>
+      <c r="R11" s="18">
+        <v>9.7916666666666666E-2</v>
+      </c>
+      <c r="S11" s="18">
+        <v>0.47152777777777777</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1">
+        <v>2</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>15</v>
+      </c>
+      <c r="P12" s="18">
+        <v>0.48541666666666666</v>
+      </c>
+      <c r="Q12" s="18">
+        <v>0</v>
+      </c>
+      <c r="R12" s="18">
+        <v>8.0555555555555561E-2</v>
+      </c>
+      <c r="S12" s="18">
+        <v>0.40486111111111112</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0</v>
+      </c>
+      <c r="U12" s="1">
+        <v>0</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>16</v>
+      </c>
+      <c r="P13" s="18">
+        <v>0.47222222222222221</v>
+      </c>
+      <c r="Q13" s="18">
+        <v>4.3749999999999997E-2</v>
+      </c>
+      <c r="R13" s="18">
+        <v>7.5694444444444439E-2</v>
+      </c>
+      <c r="S13" s="18">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="T13" s="1">
+        <v>5</v>
+      </c>
+      <c r="U13" s="1">
+        <v>7</v>
+      </c>
+      <c r="V13" s="1">
+        <v>41.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>6</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1">
+        <v>14</v>
+      </c>
+      <c r="P14" s="18">
+        <v>0.45624999999999999</v>
+      </c>
+      <c r="Q14" s="18">
+        <v>1.8055555555555554E-2</v>
+      </c>
+      <c r="R14" s="18">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="S14" s="18">
+        <v>0.4375</v>
+      </c>
+      <c r="T14" s="1">
+        <v>2</v>
+      </c>
+      <c r="U14" s="1">
+        <v>7</v>
+      </c>
+      <c r="V14" s="1">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>2</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1">
+        <v>15</v>
+      </c>
+      <c r="P15" s="18">
+        <v>0.40694444444444444</v>
+      </c>
+      <c r="Q15" s="18">
+        <v>4.3749999999999997E-2</v>
+      </c>
+      <c r="R15" s="18">
+        <v>0</v>
+      </c>
+      <c r="S15" s="18">
+        <v>0.36319444444444443</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0</v>
+      </c>
+      <c r="U15" s="1">
+        <v>0</v>
+      </c>
+      <c r="V15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>4</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>13</v>
+      </c>
+      <c r="P16" s="18">
+        <v>0.32847222222222222</v>
+      </c>
+      <c r="Q16" s="18">
+        <v>0</v>
+      </c>
+      <c r="R16" s="18">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="S16" s="18">
+        <v>0.28194444444444444</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0</v>
+      </c>
+      <c r="U16" s="1">
+        <v>2</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+      <c r="M17" s="1">
+        <v>2</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <v>15</v>
+      </c>
+      <c r="P17" s="18">
+        <v>0.49583333333333335</v>
+      </c>
+      <c r="Q17" s="18">
+        <v>3.6805555555555557E-2</v>
+      </c>
+      <c r="R17" s="18">
+        <v>8.1944444444444445E-2</v>
+      </c>
+      <c r="S17" s="18">
+        <v>0.37708333333333333</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0</v>
+      </c>
+      <c r="U17" s="1">
+        <v>0</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>2</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>2</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1</v>
+      </c>
+      <c r="N18" s="1">
+        <v>2</v>
+      </c>
+      <c r="O18" s="1">
+        <v>14</v>
+      </c>
+      <c r="P18" s="18">
+        <v>0.50069444444444444</v>
+      </c>
+      <c r="Q18" s="18">
+        <v>0.12430555555555556</v>
+      </c>
+      <c r="R18" s="18">
+        <v>0</v>
+      </c>
+      <c r="S18" s="18">
+        <v>0.37638888888888888</v>
+      </c>
+      <c r="T18" s="1">
+        <v>1</v>
+      </c>
+      <c r="U18" s="1">
+        <v>0</v>
+      </c>
+      <c r="V18" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>2</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <v>16</v>
+      </c>
+      <c r="P19" s="18">
+        <v>0.56180555555555556</v>
+      </c>
+      <c r="Q19" s="18">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="R19" s="18">
+        <v>0.10902777777777778</v>
+      </c>
+      <c r="S19" s="18">
+        <v>0.43958333333333333</v>
+      </c>
+      <c r="T19" s="1">
+        <v>0</v>
+      </c>
+      <c r="U19" s="1">
+        <v>0</v>
+      </c>
+      <c r="V19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>2</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>5</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <v>13</v>
+      </c>
+      <c r="P20" s="18">
+        <v>0.40277777777777779</v>
+      </c>
+      <c r="Q20" s="18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="R20" s="18">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="S20" s="18">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="T20" s="1">
+        <v>1</v>
+      </c>
+      <c r="U20" s="1">
+        <v>1</v>
+      </c>
+      <c r="V20" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>2</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <v>2</v>
+      </c>
+      <c r="O21" s="1">
+        <v>13</v>
+      </c>
+      <c r="P21" s="18">
+        <v>0.4</v>
+      </c>
+      <c r="Q21" s="18">
+        <v>0</v>
+      </c>
+      <c r="R21" s="18">
+        <v>0</v>
+      </c>
+      <c r="S21" s="18">
+        <v>0.4</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0</v>
+      </c>
+      <c r="U21" s="1">
+        <v>0</v>
+      </c>
+      <c r="V21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>2</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>3</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>15</v>
+      </c>
+      <c r="P22" s="18">
+        <v>0.54236111111111107</v>
+      </c>
+      <c r="Q22" s="18">
+        <v>0</v>
+      </c>
+      <c r="R22" s="18">
+        <v>6.9444444444444448E-2</v>
+      </c>
+      <c r="S22" s="18">
+        <v>0.47291666666666665</v>
+      </c>
+      <c r="T22" s="1">
+        <v>0</v>
+      </c>
+      <c r="U22" s="1">
+        <v>0</v>
+      </c>
+      <c r="V22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>3</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <v>14</v>
+      </c>
+      <c r="P23" s="18">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="Q23" s="18">
+        <v>0.18124999999999999</v>
+      </c>
+      <c r="R23" s="18">
+        <v>0</v>
+      </c>
+      <c r="S23" s="18">
+        <v>0.42291666666666666</v>
+      </c>
+      <c r="T23" s="1">
+        <v>4</v>
+      </c>
+      <c r="U23" s="1">
+        <v>3</v>
+      </c>
+      <c r="V23" s="1">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <v>2</v>
+      </c>
+      <c r="K24" s="1">
+        <v>4</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <v>2</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0</v>
+      </c>
+      <c r="O24" s="1">
+        <v>13</v>
+      </c>
+      <c r="P24" s="18">
+        <v>0.37361111111111112</v>
+      </c>
+      <c r="Q24" s="18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="R24" s="18">
+        <v>0</v>
+      </c>
+      <c r="S24" s="18">
+        <v>0.34861111111111109</v>
+      </c>
+      <c r="T24" s="1">
+        <v>0</v>
+      </c>
+      <c r="U24" s="1">
+        <v>0</v>
+      </c>
+      <c r="V24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <v>3</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0</v>
+      </c>
+      <c r="O25" s="1">
+        <v>8</v>
+      </c>
+      <c r="P25" s="18">
+        <v>0.25277777777777777</v>
+      </c>
+      <c r="Q25" s="18">
+        <v>0</v>
+      </c>
+      <c r="R25" s="18">
+        <v>0</v>
+      </c>
+      <c r="S25" s="18">
+        <v>0.25277777777777777</v>
+      </c>
+      <c r="T25" s="1">
+        <v>0</v>
+      </c>
+      <c r="U25" s="1">
+        <v>0</v>
+      </c>
+      <c r="V25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <v>16</v>
+      </c>
+      <c r="P26" s="18">
+        <v>0.59097222222222223</v>
+      </c>
+      <c r="Q26" s="18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="R26" s="18">
+        <v>7.013888888888889E-2</v>
+      </c>
+      <c r="S26" s="18">
+        <v>0.49583333333333335</v>
+      </c>
+      <c r="T26" s="1">
+        <v>0</v>
+      </c>
+      <c r="U26" s="1">
+        <v>0</v>
+      </c>
+      <c r="V26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>3</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0</v>
+      </c>
+      <c r="O27" s="1">
+        <v>17</v>
+      </c>
+      <c r="P27" s="18">
+        <v>0.60972222222222228</v>
+      </c>
+      <c r="Q27" s="18">
+        <v>0.18124999999999999</v>
+      </c>
+      <c r="R27" s="18">
+        <v>0</v>
+      </c>
+      <c r="S27" s="18">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="T27" s="1">
+        <v>0</v>
+      </c>
+      <c r="U27" s="1">
+        <v>0</v>
+      </c>
+      <c r="V27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>4</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <v>3</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+      <c r="O28" s="1">
+        <v>11</v>
+      </c>
+      <c r="P28" s="18">
+        <v>0.39444444444444443</v>
+      </c>
+      <c r="Q28" s="18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="R28" s="18">
+        <v>0</v>
+      </c>
+      <c r="S28" s="18">
+        <v>0.36944444444444446</v>
+      </c>
+      <c r="T28" s="1">
+        <v>0</v>
+      </c>
+      <c r="U28" s="1">
+        <v>0</v>
+      </c>
+      <c r="V28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G29" s="1">
+        <v>6</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
+        <v>2</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1">
+        <v>13</v>
+      </c>
+      <c r="P29" s="18">
+        <v>0.58958333333333335</v>
+      </c>
+      <c r="Q29" s="18">
+        <v>0.18124999999999999</v>
+      </c>
+      <c r="R29" s="18">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="S29" s="18">
+        <v>0.40138888888888891</v>
+      </c>
+      <c r="T29" s="1">
+        <v>12</v>
+      </c>
+      <c r="U29" s="1">
+        <v>7</v>
+      </c>
+      <c r="V29" s="1">
+        <v>63.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <v>2</v>
+      </c>
+      <c r="M30" s="1">
+        <v>1</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0</v>
+      </c>
+      <c r="O30" s="1">
+        <v>17</v>
+      </c>
+      <c r="P30" s="18">
+        <v>0.5395833333333333</v>
+      </c>
+      <c r="Q30" s="18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="R30" s="18">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="S30" s="18">
+        <v>0.41736111111111113</v>
+      </c>
+      <c r="T30" s="1">
+        <v>0</v>
+      </c>
+      <c r="U30" s="1">
+        <v>0</v>
+      </c>
+      <c r="V30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1">
+        <v>4</v>
+      </c>
+      <c r="M31" s="1">
+        <v>0</v>
+      </c>
+      <c r="N31" s="1">
+        <v>0</v>
+      </c>
+      <c r="O31" s="1">
+        <v>10</v>
+      </c>
+      <c r="P31" s="18">
+        <v>0.32222222222222224</v>
+      </c>
+      <c r="Q31" s="18">
+        <v>0</v>
+      </c>
+      <c r="R31" s="18">
+        <v>6.7361111111111108E-2</v>
+      </c>
+      <c r="S31" s="18">
+        <v>0.25486111111111109</v>
+      </c>
+      <c r="T31" s="1">
+        <v>0</v>
+      </c>
+      <c r="U31" s="1">
+        <v>0</v>
+      </c>
+      <c r="V31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1</v>
+      </c>
+      <c r="H32" s="1">
+        <v>2</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
+        <v>2</v>
+      </c>
+      <c r="M32" s="1">
+        <v>4</v>
+      </c>
+      <c r="N32" s="1">
+        <v>1</v>
+      </c>
+      <c r="O32" s="1">
+        <v>12</v>
+      </c>
+      <c r="P32" s="18">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="Q32" s="18">
+        <v>0</v>
+      </c>
+      <c r="R32" s="18">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="S32" s="18">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="T32" s="1">
+        <v>3</v>
+      </c>
+      <c r="U32" s="1">
+        <v>3</v>
+      </c>
+      <c r="V32" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0</v>
+      </c>
+      <c r="O33" s="1">
+        <v>13</v>
+      </c>
+      <c r="P33" s="18">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="Q33" s="18">
+        <v>0.18124999999999999</v>
+      </c>
+      <c r="R33" s="18">
+        <v>6.7361111111111108E-2</v>
+      </c>
+      <c r="S33" s="18">
+        <v>0.25486111111111109</v>
+      </c>
+      <c r="T33" s="1">
+        <v>0</v>
+      </c>
+      <c r="U33" s="1">
+        <v>2</v>
+      </c>
+      <c r="V33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
+        <v>5</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0</v>
+      </c>
+      <c r="O34" s="1">
+        <v>10</v>
+      </c>
+      <c r="P34" s="18">
+        <v>0.2388888888888889</v>
+      </c>
+      <c r="Q34" s="18">
+        <v>0</v>
+      </c>
+      <c r="R34" s="18">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="S34" s="18">
+        <v>0.21666666666666667</v>
+      </c>
+      <c r="T34" s="1">
+        <v>5</v>
+      </c>
+      <c r="U34" s="1">
+        <v>2</v>
+      </c>
+      <c r="V34" s="1">
+        <v>71.400000000000006</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1">
+        <v>3</v>
+      </c>
+      <c r="M35" s="1">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1">
+        <v>0</v>
+      </c>
+      <c r="O35" s="1">
+        <v>14</v>
+      </c>
+      <c r="P35" s="18">
+        <v>0.47152777777777777</v>
+      </c>
+      <c r="Q35" s="18">
+        <v>0</v>
+      </c>
+      <c r="R35" s="18">
+        <v>9.6527777777777782E-2</v>
+      </c>
+      <c r="S35" s="18">
+        <v>0.375</v>
+      </c>
+      <c r="T35" s="1">
+        <v>0</v>
+      </c>
+      <c r="U35" s="1">
+        <v>0</v>
+      </c>
+      <c r="V35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+      <c r="F36" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>2</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1">
+        <v>4</v>
+      </c>
+      <c r="M36" s="1">
+        <v>1</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+      <c r="O36" s="1">
+        <v>13</v>
+      </c>
+      <c r="P36" s="18">
+        <v>0.35902777777777778</v>
+      </c>
+      <c r="Q36" s="18">
+        <v>0</v>
+      </c>
+      <c r="R36" s="18">
+        <v>6.5277777777777782E-2</v>
+      </c>
+      <c r="S36" s="18">
+        <v>0.29375000000000001</v>
+      </c>
+      <c r="T36" s="1">
+        <v>0</v>
+      </c>
+      <c r="U36" s="1">
+        <v>0</v>
+      </c>
+      <c r="V36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>2</v>
+      </c>
+      <c r="H37" s="1">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1">
+        <v>1</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0</v>
+      </c>
+      <c r="L37" s="1">
+        <v>2</v>
+      </c>
+      <c r="M37" s="1">
+        <v>1</v>
+      </c>
+      <c r="N37" s="1">
+        <v>0</v>
+      </c>
+      <c r="O37" s="1">
+        <v>14</v>
+      </c>
+      <c r="P37" s="18">
+        <v>0.59236111111111112</v>
+      </c>
+      <c r="Q37" s="18">
+        <v>0.18124999999999999</v>
+      </c>
+      <c r="R37" s="18">
+        <v>0</v>
+      </c>
+      <c r="S37" s="18">
+        <v>0.41111111111111109</v>
+      </c>
+      <c r="T37" s="1">
+        <v>0</v>
+      </c>
+      <c r="U37" s="1">
+        <v>0</v>
+      </c>
+      <c r="V37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V19">
+    <sortCondition ref="A2:A19"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="I3" sqref="I3:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38367,11 +40910,11 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38392,24 +40935,145 @@
       <c r="C1" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="O1" s="6" t="s">
         <v>426</v>
       </c>
     </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="H2" s="1">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="19">
+        <v>1.663888888888889</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="H3" s="1">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="19">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O1" location="'Scores (4-24-24)'!A1" display="HOME"/>
+    <hyperlink ref="O1" location="'Scores (4-24-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:F3"/>
+      <selection activeCell="M8" sqref="M8:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38433,7 +41097,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -38462,8 +41126,12 @@
         <v>6</v>
       </c>
       <c r="N1" s="21"/>
-    </row>
-    <row r="2" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="21"/>
+    </row>
+    <row r="2" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
@@ -38506,8 +41174,14 @@
       <c r="N2" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>380</v>
       </c>
@@ -38550,8 +41224,14 @@
       <c r="N3" s="1" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>382</v>
       </c>
@@ -38594,8 +41274,14 @@
       <c r="N4" s="1" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>384</v>
       </c>
@@ -38620,39 +41306,49 @@
       <c r="N5" s="1" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O5" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H8" s="21"/>
       <c r="I8" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J8" s="21"/>
       <c r="K8" s="20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L8" s="21"/>
       <c r="M8" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N8" s="21"/>
-    </row>
-    <row r="9" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="P8" s="21"/>
+    </row>
+    <row r="9" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>25</v>
       </c>
@@ -38695,197 +41391,154 @@
       <c r="N9" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>379</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>379</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>379</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>379</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>379</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>379</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>379</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>379</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>379</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>379</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>379</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>379</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>379</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>379</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>379</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>379</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>379</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>379</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="21"/>
-    </row>
-    <row r="15" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="B18" s="1" t="s">
         <v>379</v>
       </c>
     </row>
@@ -38893,15 +41546,15 @@
   <mergeCells count="16">
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="I8:J8"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="M8:N8"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="O1:P1"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
@@ -38914,7 +41567,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -38932,7 +41585,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -38963,14 +41616,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O1" location="'Scores (4-25-24)'!A1" display="HOME"/>
+    <hyperlink ref="O1" location="'Scores (4-25-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -38988,7 +41641,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -39019,14 +41672,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O1" location="'Scores (4-26-24)'!A1" display="HOME"/>
+    <hyperlink ref="O1" location="'Scores (4-26-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1C00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -39136,21 +41789,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E10" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A11" location="'Offense (10-10-23)'!A1" display="Offense"/>
-    <hyperlink ref="A12" location="'Goalies (10-10-23)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A11" location="'Offense (10-10-23)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A12" location="'Goalies (10-10-23)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -39163,7 +41816,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -39181,7 +41834,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -39212,14 +41865,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O1" location="'Scores (4-27-24)'!A1" display="HOME"/>
+    <hyperlink ref="O1" location="'Scores (4-27-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -39237,7 +41890,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -39268,14 +41921,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O1" location="'Scores (4-28-24)'!A1" display="HOME"/>
+    <hyperlink ref="O1" location="'Scores (4-28-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-2000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -39293,7 +41946,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -39324,14 +41977,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O1" location="'Scores (4-29-24)'!A1" display="HOME"/>
+    <hyperlink ref="O1" location="'Scores (4-29-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -39421,21 +42074,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A5" location="'Offense (4-20-24)'!A1" display="Offense"/>
-    <hyperlink ref="A6" location="'Goalies (4-20-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="A5" location="'Offense (4-20-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="A6" location="'Goalies (4-20-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -39448,7 +42101,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -39566,21 +42219,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A7" location="'Offense (4-21-24)'!A1" display="Offense"/>
-    <hyperlink ref="A8" location="'Goalies (4-21-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="A7" location="'Offense (4-21-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="A8" location="'Goalies (4-21-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -39593,7 +42246,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -39711,21 +42364,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A7" location="'Offense (4-22-24)'!A1" display="Offense"/>
-    <hyperlink ref="A8" location="'Goalies (4-22-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="A7" location="'Offense (4-22-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="A8" location="'Goalies (4-22-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -39738,11 +42391,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39859,21 +42512,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A7" location="'Offense (4-23-24)'!A1" display="Offense"/>
-    <hyperlink ref="A8" location="'Goalies (4-23-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="A7" location="'Offense (4-23-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="A8" location="'Goalies (4-23-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -39886,11 +42539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39937,11 +42590,15 @@
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="9">
+        <v>4</v>
+      </c>
       <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -39978,21 +42635,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E5" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A6" location="'Offense (4-24-24)'!A1" display="Offense"/>
-    <hyperlink ref="A7" location="'Goalies (4-24-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="A6" location="'Offense (4-24-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="A7" location="'Goalies (4-24-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -40005,7 +42662,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -40087,21 +42744,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A5" location="'Offense (4-25-24)'!A1" display="Offense"/>
-    <hyperlink ref="A6" location="'Goalies (4-25-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="A5" location="'Offense (4-25-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="A6" location="'Goalies (4-25-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Updated Playoff Box Scores, Brackets
Data Input to EOD 5/1/24
</commit_message>
<xml_diff>
--- a/2024/Playoffs/BoxScores.xlsx
+++ b/2024/Playoffs/BoxScores.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LunchProjects\GitHub\NHLStats\2024\Playoffs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\NHLStats\2024\Playoffs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290D7C3A-6B8B-4A66-AF2C-789368990599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="9" activeTab="15"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="10" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -28,36 +29,39 @@
     <sheet name="Scores (4-30-24)" sheetId="38" r:id="rId14"/>
     <sheet name="Scores (5-1-24)" sheetId="43" r:id="rId15"/>
     <sheet name="Scores (5-2-24)" sheetId="46" r:id="rId16"/>
-    <sheet name="Offense (4-20-24)" sheetId="6" r:id="rId17"/>
-    <sheet name="Goalies (4-20-24)" sheetId="7" r:id="rId18"/>
-    <sheet name="Offense (4-21-24)" sheetId="9" r:id="rId19"/>
-    <sheet name="Goalies (4-21-24)" sheetId="8" r:id="rId20"/>
-    <sheet name="Offense (4-22-24)" sheetId="13" r:id="rId21"/>
-    <sheet name="Goalies (4-22-24)" sheetId="14" r:id="rId22"/>
-    <sheet name="Offense (4-23-24)" sheetId="15" r:id="rId23"/>
-    <sheet name="Goalies (4-23-24)" sheetId="16" r:id="rId24"/>
-    <sheet name="Offense (4-24-24)" sheetId="17" r:id="rId25"/>
-    <sheet name="Goalies (4-24-24)" sheetId="18" r:id="rId26"/>
-    <sheet name="Offense (4-25-24)" sheetId="19" r:id="rId27"/>
-    <sheet name="Goalies (4-25-24)" sheetId="20" r:id="rId28"/>
-    <sheet name="Offense (4-26-24)" sheetId="21" r:id="rId29"/>
-    <sheet name="Goalies (4-26-24)" sheetId="22" r:id="rId30"/>
-    <sheet name="Offense (4-27-24)" sheetId="23" r:id="rId31"/>
-    <sheet name="Goalies (4-27-24)" sheetId="24" r:id="rId32"/>
-    <sheet name="Offense (4-28-24)" sheetId="25" r:id="rId33"/>
-    <sheet name="Goalies (4-28-24)" sheetId="26" r:id="rId34"/>
-    <sheet name="Offense (4-29-24)" sheetId="27" r:id="rId35"/>
-    <sheet name="Goalies (4-29-24)" sheetId="28" r:id="rId36"/>
-    <sheet name="Offense (4-30-24)" sheetId="36" r:id="rId37"/>
-    <sheet name="Goalies (4-30-24)" sheetId="37" r:id="rId38"/>
-    <sheet name="Offense (5-1-24)" sheetId="40" r:id="rId39"/>
-    <sheet name="Goalies (5-1-24)" sheetId="39" r:id="rId40"/>
-    <sheet name="Offense (5-2-24)" sheetId="42" r:id="rId41"/>
-    <sheet name="Rosters (Offense)" sheetId="4" r:id="rId42"/>
+    <sheet name="Scores (5-3-24)" sheetId="49" r:id="rId17"/>
+    <sheet name="Offense (4-20-24)" sheetId="6" r:id="rId18"/>
+    <sheet name="Goalies (4-20-24)" sheetId="7" r:id="rId19"/>
+    <sheet name="Offense (4-21-24)" sheetId="9" r:id="rId20"/>
+    <sheet name="Goalies (4-21-24)" sheetId="8" r:id="rId21"/>
+    <sheet name="Offense (4-22-24)" sheetId="13" r:id="rId22"/>
+    <sheet name="Goalies (4-22-24)" sheetId="14" r:id="rId23"/>
+    <sheet name="Offense (4-23-24)" sheetId="15" r:id="rId24"/>
+    <sheet name="Goalies (4-23-24)" sheetId="16" r:id="rId25"/>
+    <sheet name="Offense (4-24-24)" sheetId="17" r:id="rId26"/>
+    <sheet name="Goalies (4-24-24)" sheetId="18" r:id="rId27"/>
+    <sheet name="Offense (4-25-24)" sheetId="19" r:id="rId28"/>
+    <sheet name="Goalies (4-25-24)" sheetId="20" r:id="rId29"/>
+    <sheet name="Offense (4-26-24)" sheetId="21" r:id="rId30"/>
+    <sheet name="Goalies (4-26-24)" sheetId="22" r:id="rId31"/>
+    <sheet name="Offense (4-27-24)" sheetId="23" r:id="rId32"/>
+    <sheet name="Goalies (4-27-24)" sheetId="24" r:id="rId33"/>
+    <sheet name="Offense (4-28-24)" sheetId="25" r:id="rId34"/>
+    <sheet name="Goalies (4-28-24)" sheetId="26" r:id="rId35"/>
+    <sheet name="Offense (4-29-24)" sheetId="27" r:id="rId36"/>
+    <sheet name="Goalies (4-29-24)" sheetId="28" r:id="rId37"/>
+    <sheet name="Offense (4-30-24)" sheetId="36" r:id="rId38"/>
+    <sheet name="Goalies (4-30-24)" sheetId="37" r:id="rId39"/>
+    <sheet name="Offense (5-1-24)" sheetId="40" r:id="rId40"/>
+    <sheet name="Goalies (5-1-24)" sheetId="39" r:id="rId41"/>
+    <sheet name="Offense (5-2-24)" sheetId="42" r:id="rId42"/>
     <sheet name="Goalies (5-2-24)" sheetId="41" r:id="rId43"/>
-    <sheet name="Rosters (Goalies)" sheetId="5" r:id="rId44"/>
-    <sheet name="Offense (5-3-24)" sheetId="44" r:id="rId45"/>
+    <sheet name="Offense (5-3-24)" sheetId="44" r:id="rId44"/>
+    <sheet name="Rosters (Offense)" sheetId="4" r:id="rId45"/>
     <sheet name="Goalies (5-3-24)" sheetId="45" r:id="rId46"/>
+    <sheet name="Rosters (Goalies)" sheetId="5" r:id="rId47"/>
+    <sheet name="Offense (5-4-24)" sheetId="47" r:id="rId48"/>
+    <sheet name="Goalies (5-4-24)" sheetId="48" r:id="rId49"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -69,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5781" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5944" uniqueCount="469">
   <si>
     <t>Boston Bruins</t>
   </si>
@@ -1474,11 +1478,14 @@
   <si>
     <t>May 2nd 2024</t>
   </si>
+  <si>
+    <t>May 3rd 2024</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -2042,11 +2049,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2170,7 +2177,9 @@
       <c r="A15" s="14">
         <v>45414</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="16" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
@@ -2353,18 +2362,19 @@
     <mergeCell ref="A13:B13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" location="'Scores (4-20-24)'!A1" display="Scores"/>
-    <hyperlink ref="B3" location="'Scores (4-21-24)'!A1" display="Scores"/>
-    <hyperlink ref="B4" location="'Scores (4-22-24)'!A1" display="Scores"/>
-    <hyperlink ref="B5" location="'Scores (4-23-24)'!A1" display="Scores"/>
-    <hyperlink ref="B6" location="'Scores (4-24-24)'!A1" display="Scores"/>
-    <hyperlink ref="B7" location="'Scores (4-25-24)'!A1" display="Scores"/>
-    <hyperlink ref="B8" location="'Scores (4-26-24)'!A1" display="Scores"/>
-    <hyperlink ref="B9" location="'Scores (4-27-24)'!A1" display="Scores"/>
-    <hyperlink ref="B10" location="'Scores (4-28-24)'!A1" display="Scores"/>
-    <hyperlink ref="B11" location="'Scores (4-29-24)'!A1" display="Scores"/>
-    <hyperlink ref="B12" location="'Scores (4-30-24)'!A1" display="Scores"/>
-    <hyperlink ref="B14" location="'Scores (5-1-24)'!A1" display="Scores"/>
+    <hyperlink ref="B2" location="'Scores (4-20-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" location="'Scores (4-21-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" location="'Scores (4-22-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" location="'Scores (4-23-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" location="'Scores (4-24-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" location="'Scores (4-25-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" location="'Scores (4-26-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" location="'Scores (4-27-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" location="'Scores (4-28-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" location="'Scores (4-29-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" location="'Scores (4-30-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B14" location="'Scores (5-1-24)'!A1" display="Scores" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B15" location="'Scores (5-2-24)'!A1" display="Scores" xr:uid="{B6DE971B-0731-41D2-BF5F-80348546DD2A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2372,7 +2382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2490,21 +2500,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A7" location="'Offense (4-26-24)'!A1" display="Offense"/>
-    <hyperlink ref="A8" location="'Goalies (4-26-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="A7" location="'Offense (4-26-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="A8" location="'Goalies (4-26-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -2517,7 +2527,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2644,24 +2654,24 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E6" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3" xr:uid="{00000000-0002-0000-0A00-000001000000}">
       <formula1>$AA$1:$AA$3</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A7" location="'Offense (4-27-24)'!A1" display="Offense"/>
-    <hyperlink ref="A8" location="'Goalies (4-27-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="A7" location="'Offense (4-27-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="A8" location="'Goalies (4-27-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000002000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -2674,7 +2684,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2795,21 +2805,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A7" location="'Offense (4-28-24)'!A1" display="Offense"/>
-    <hyperlink ref="A8" location="'Goalies (4-28-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="A7" location="'Offense (4-28-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="A8" location="'Goalies (4-28-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0B00-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -2822,11 +2832,11 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2912,21 +2922,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A5" location="'Offense (4-29-24)'!A1" display="Offense"/>
-    <hyperlink ref="A6" location="'Goalies (4-29-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="A5" location="'Offense (4-29-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
+    <hyperlink ref="A6" location="'Goalies (4-29-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0C00-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -2939,7 +2949,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3060,21 +3070,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0D00-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A7" location="'Offense (4-30-24)'!A1" display="Offense"/>
-    <hyperlink ref="A8" location="'Goalies (4-30-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="A7" location="'Offense (4-30-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
+    <hyperlink ref="A8" location="'Goalies (4-30-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0D00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0D00-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -3087,7 +3097,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3177,21 +3187,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4" xr:uid="{00000000-0002-0000-0E00-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A5" location="'Offense (5-1-24)'!A1" display="Offense"/>
-    <hyperlink ref="A6" location="'Goalies (5-1-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="A5" location="'Offense (5-1-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0E00-000001000000}"/>
+    <hyperlink ref="A6" location="'Goalies (5-1-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0E00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0E00-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -3204,8 +3214,111 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AA5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="23" t="s">
+        <v>467</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3" xr:uid="{00000000-0002-0000-0F00-000000000000}">
+      <formula1>$AA$1:$AA$2</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="A4" location="'Offense (5-2-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0F00-000001000000}"/>
+    <hyperlink ref="A5" location="'Goalies (5-2-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0F00-000002000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0F00-000001000000}">
+          <x14:formula1>
+            <xm:f>Teams!$C$2:$C$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>A3 C3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07234016-960A-4FAB-A82F-2E92F876705F}">
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -3222,7 +3335,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="23" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -3251,23 +3364,33 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="3" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3276,25 +3399,25 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4" xr:uid="{FBDFB806-3C40-4D83-9034-AA09C8BDED29}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A4" location="'Offense (5-2-24)'!A1" display="Offense"/>
-    <hyperlink ref="A5" location="'Goalies (5-2-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{9284FE46-3BC8-40EC-BBA8-5B0D51C0FFAE}"/>
+    <hyperlink ref="A5" location="'Offense (5-3-24)'!A1" display="Offense" xr:uid="{9C832D34-234A-4D87-A791-9A27BB0EE788}"/>
+    <hyperlink ref="A6" location="'Goalies (5-3-24)'!A1" display="Goalies" xr:uid="{49277994-6DBA-4964-A2A6-AE462D17AA9E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{86A08A4E-E92E-4737-AAC0-E92D98F2B76A}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
-          <xm:sqref>A3 C3</xm:sqref>
+          <xm:sqref>C3:C4 A3:A4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3302,8 +3425,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:U73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7850,19 +7973,19 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:U187">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U187">
     <sortCondition ref="C2:C187"/>
     <sortCondition ref="A2:A187"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-20-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (4-20-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8071,18 +8194,282 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L5">
     <sortCondition ref="C2:C5"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-20-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-20-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="M39" s="4"/>
+    </row>
+    <row r="40" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="M40" s="4"/>
+    </row>
+    <row r="41" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="M41" s="4"/>
+    </row>
+    <row r="42" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="M42" s="4"/>
+    </row>
+    <row r="43" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="M43" s="4"/>
+    </row>
+    <row r="44" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I44" s="4"/>
+      <c r="M44" s="4"/>
+    </row>
+    <row r="45" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I45" s="4"/>
+      <c r="M45" s="4"/>
+    </row>
+    <row r="46" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="M46" s="4"/>
+    </row>
+    <row r="48" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="M48" s="4"/>
+    </row>
+    <row r="49" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="I49" s="4"/>
+      <c r="M49" s="4"/>
+    </row>
+    <row r="50" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="M50" s="4"/>
+    </row>
+    <row r="51" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H51" s="4"/>
+      <c r="M51" s="4"/>
+    </row>
+    <row r="52" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="M52" s="4"/>
+    </row>
+    <row r="53" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H53" s="4"/>
+      <c r="M53" s="4"/>
+    </row>
+    <row r="54" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="M54" s="4"/>
+    </row>
+    <row r="55" spans="8:13" x14ac:dyDescent="0.25">
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="M55" s="4"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B9">
+    <sortCondition ref="B2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:T145"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17089,7 +17476,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:X204">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X204">
     <sortCondition ref="C2:C204"/>
     <sortCondition ref="A2:A204"/>
   </sortState>
@@ -17097,272 +17484,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M55"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="M39" s="4"/>
-    </row>
-    <row r="40" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="M40" s="4"/>
-    </row>
-    <row r="41" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="M41" s="4"/>
-    </row>
-    <row r="42" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="M42" s="4"/>
-    </row>
-    <row r="43" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="M43" s="4"/>
-    </row>
-    <row r="44" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="I44" s="4"/>
-      <c r="M44" s="4"/>
-    </row>
-    <row r="45" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="I45" s="4"/>
-      <c r="M45" s="4"/>
-    </row>
-    <row r="46" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="M46" s="4"/>
-    </row>
-    <row r="48" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="M48" s="4"/>
-    </row>
-    <row r="49" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="I49" s="4"/>
-      <c r="M49" s="4"/>
-    </row>
-    <row r="50" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="M50" s="4"/>
-    </row>
-    <row r="51" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H51" s="4"/>
-      <c r="M51" s="4"/>
-    </row>
-    <row r="52" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="M52" s="4"/>
-    </row>
-    <row r="53" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H53" s="4"/>
-      <c r="M53" s="4"/>
-    </row>
-    <row r="54" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="M54" s="4"/>
-    </row>
-    <row r="55" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
-      <c r="M55" s="4"/>
-    </row>
-  </sheetData>
-  <sortState ref="B2:B9">
-    <sortCondition ref="B2"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17723,18 +17846,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L9">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L9">
     <sortCondition ref="C2:C9"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-21-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-21-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:U145"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26744,20 +26867,20 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:X263">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X263">
     <sortCondition ref="C2:C263"/>
     <sortCondition ref="A2:A263"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-22-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (4-22-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27118,18 +27241,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:N9">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N9">
     <sortCondition ref="C2:C9"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-22-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-22-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:U145"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -36139,20 +36262,20 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:X263">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X263">
     <sortCondition ref="C2:C263"/>
     <sortCondition ref="A2:A263"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-23-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (4-23-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36513,18 +36636,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:N9">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N9">
     <sortCondition ref="C2:C9"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-23-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-23-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:U109"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -43302,18 +43425,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A74:V91">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A74:V91">
     <sortCondition ref="A74"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-24-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (4-24-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -43598,18 +43721,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L7">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L7">
     <sortCondition ref="C2:C7"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-24-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-24-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:U73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -48156,18 +48279,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:U19">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U19">
     <sortCondition ref="A2:A19"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-25-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (4-25-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -48415,14 +48538,151 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-25-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-25-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AA12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="23" t="s">
+        <v>415</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E10" xr:uid="{00000000-0002-0000-0200-000000000000}">
+      <formula1>$AA$1:$AA$2</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A11" location="'Offense (10-10-23)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A12" location="'Goalies (10-10-23)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
+          <x14:formula1>
+            <xm:f>Teams!$C$2:$C$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>A3:A10 C3:C10</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:U145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -57433,155 +57693,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:U19">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U19">
     <sortCondition ref="A2:A19"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-26-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (4-26-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1C00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
-        <v>415</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E10">
-      <formula1>$AA$1:$AA$2</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A11" location="'Offense (10-10-23)'!A1" display="Offense"/>
-    <hyperlink ref="A12" location="'Goalies (10-10-23)'!A1" display="Goalies"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Teams!$C$2:$C$17</xm:f>
-          </x14:formula1>
-          <xm:sqref>A3:A10 C3:C10</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -57942,18 +58065,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L9">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L9">
     <sortCondition ref="C2:C9"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-26-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-26-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:U145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -66964,18 +67087,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A110:U127">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A110:U127">
     <sortCondition ref="A110:A127"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-27-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (4-27-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -67374,18 +67497,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L10">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L10">
     <sortCondition ref="C2:C10"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-27-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-27-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-1F00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:U145"/>
   <sheetViews>
     <sheetView topLeftCell="A127" workbookViewId="0">
@@ -76396,19 +76519,19 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:V382">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V382">
     <sortCondition ref="C2:C382"/>
     <sortCondition ref="A2:A382"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-28-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (4-28-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-2000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -76807,18 +76930,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:N10">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N10">
     <sortCondition ref="C2:C10"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-28-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-28-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:U73"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -81363,18 +81486,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:V19">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V19">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-29-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (4-29-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -81581,18 +81704,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:N5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N5">
     <sortCondition ref="C2:C5"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-29-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-29-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-2300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:U145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -90603,19 +90726,19 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:V380">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V380">
     <sortCondition ref="C2:C380"/>
     <sortCondition ref="A2:A380"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (4-30-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (4-30-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-2400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -90976,19 +91099,136 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:N9">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N9">
     <sortCondition ref="C2:C9"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (4-30-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (4-30-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-2500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AA6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="23" t="s">
+        <v>415</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4" xr:uid="{00000000-0002-0000-0300-000000000000}">
+      <formula1>$AA$1:$AA$2</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="A5" location="'Offense (4-20-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="A6" location="'Goalies (4-20-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
+          <x14:formula1>
+            <xm:f>Teams!$C$2:$C$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:C4 A3:A4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:U73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -95535,135 +95775,18 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:V19">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V19">
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="U1" location="'Scores (5-1-24)'!A1" display="HOME"/>
+    <hyperlink ref="U1" location="'Scores (5-1-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-2600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
-        <v>415</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4">
-      <formula1>$AA$1:$AA$2</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A5" location="'Offense (4-20-24)'!A1" display="Offense"/>
-    <hyperlink ref="A6" location="'Goalies (4-20-24)'!A1" display="Goalies"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Teams!$C$2:$C$17</xm:f>
-          </x14:formula1>
-          <xm:sqref>C3:C4 A3:A4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -95872,19 +95995,2486 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:N5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N5">
     <sortCondition ref="C2:C5"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="M1" location="'Scores (5-1-24)'!A1" display="HOME"/>
+    <hyperlink ref="M1" location="'Scores (5-1-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-2700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+  <dimension ref="A1:U37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
+    <col min="4" max="22" width="9.140625" style="1"/>
+    <col min="23" max="23" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>25</v>
+      </c>
+      <c r="P2" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="17">
+        <v>0.13680555555555557</v>
+      </c>
+      <c r="R2" s="17">
+        <v>0.66319444444444442</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>2</v>
+      </c>
+      <c r="L3" s="1">
+        <v>6</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>26</v>
+      </c>
+      <c r="P3" s="17">
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="Q3" s="17">
+        <v>4.2361111111111113E-2</v>
+      </c>
+      <c r="R3" s="17">
+        <v>0.68611111111111112</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>9</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>28</v>
+      </c>
+      <c r="P4" s="17">
+        <v>4.027777777777778E-2</v>
+      </c>
+      <c r="Q4" s="17">
+        <v>9.4444444444444442E-2</v>
+      </c>
+      <c r="R4" s="17">
+        <v>0.62430555555555556</v>
+      </c>
+      <c r="S4" s="1">
+        <v>8</v>
+      </c>
+      <c r="T4" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>11</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>3</v>
+      </c>
+      <c r="O5" s="1">
+        <v>32</v>
+      </c>
+      <c r="P5" s="17">
+        <v>3.6805555555555557E-2</v>
+      </c>
+      <c r="Q5" s="17">
+        <v>0.11388888888888889</v>
+      </c>
+      <c r="R5" s="17">
+        <v>0.95277777777777772</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>4</v>
+      </c>
+      <c r="L6" s="1">
+        <v>3</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
+        <v>29</v>
+      </c>
+      <c r="P6" s="17">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="Q6" s="17">
+        <v>0</v>
+      </c>
+      <c r="R6" s="17">
+        <v>0.78194444444444444</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>3</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>2</v>
+      </c>
+      <c r="O7" s="1">
+        <v>27</v>
+      </c>
+      <c r="P7" s="17">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="Q7" s="17">
+        <v>0.13263888888888889</v>
+      </c>
+      <c r="R7" s="17">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>3</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1</v>
+      </c>
+      <c r="O8" s="1">
+        <v>21</v>
+      </c>
+      <c r="P8" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="17">
+        <v>8.819444444444445E-2</v>
+      </c>
+      <c r="R8" s="17">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="S8" s="1">
+        <v>3</v>
+      </c>
+      <c r="T8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>4</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1</v>
+      </c>
+      <c r="O9" s="1">
+        <v>18</v>
+      </c>
+      <c r="P9" s="17">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="Q9" s="17">
+        <v>9.0277777777777769E-3</v>
+      </c>
+      <c r="R9" s="17">
+        <v>0.42222222222222222</v>
+      </c>
+      <c r="S9" s="1">
+        <v>1</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>8</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>2</v>
+      </c>
+      <c r="O10" s="1">
+        <v>15</v>
+      </c>
+      <c r="P10" s="17">
+        <v>3.4027777777777775E-2</v>
+      </c>
+      <c r="Q10" s="17">
+        <v>0</v>
+      </c>
+      <c r="R10" s="17">
+        <v>0.3659722222222222</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>6</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>28</v>
+      </c>
+      <c r="P11" s="17">
+        <v>3.8194444444444448E-2</v>
+      </c>
+      <c r="Q11" s="17">
+        <v>8.819444444444445E-2</v>
+      </c>
+      <c r="R11" s="17">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>2</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>17</v>
+      </c>
+      <c r="P12" s="17">
+        <v>4.2361111111111113E-2</v>
+      </c>
+      <c r="Q12" s="17">
+        <v>0</v>
+      </c>
+      <c r="R12" s="17">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>19</v>
+      </c>
+      <c r="P13" s="17">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="Q13" s="17">
+        <v>0</v>
+      </c>
+      <c r="R13" s="17">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3</v>
+      </c>
+      <c r="H14" s="1">
+        <v>4</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1">
+        <v>25</v>
+      </c>
+      <c r="P14" s="17">
+        <v>3.6805555555555557E-2</v>
+      </c>
+      <c r="Q14" s="17">
+        <v>0</v>
+      </c>
+      <c r="R14" s="17">
+        <v>0.7319444444444444</v>
+      </c>
+      <c r="S14" s="1">
+        <v>3</v>
+      </c>
+      <c r="T14" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1">
+        <v>28</v>
+      </c>
+      <c r="P15" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="17">
+        <v>0</v>
+      </c>
+      <c r="R15" s="17">
+        <v>0.90069444444444446</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>17</v>
+      </c>
+      <c r="P16" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="17">
+        <v>0</v>
+      </c>
+      <c r="R16" s="17">
+        <v>0.37638888888888888</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <v>3</v>
+      </c>
+      <c r="O17" s="1">
+        <v>21</v>
+      </c>
+      <c r="P17" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="17">
+        <v>0.11666666666666667</v>
+      </c>
+      <c r="R17" s="17">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>5</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>26</v>
+      </c>
+      <c r="P18" s="17">
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="Q18" s="17">
+        <v>0.1076388888888889</v>
+      </c>
+      <c r="R18" s="17">
+        <v>0.65763888888888888</v>
+      </c>
+      <c r="S18" s="1">
+        <v>1</v>
+      </c>
+      <c r="T18" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>5</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <v>22</v>
+      </c>
+      <c r="P19" s="17">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="Q19" s="17">
+        <v>7.013888888888889E-2</v>
+      </c>
+      <c r="R19" s="17">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="S19" s="1">
+        <v>4</v>
+      </c>
+      <c r="T19" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>3</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <v>18</v>
+      </c>
+      <c r="P20" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="17">
+        <v>2.1527777777777778E-2</v>
+      </c>
+      <c r="R20" s="17">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="S20" s="1">
+        <v>0</v>
+      </c>
+      <c r="T20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>18</v>
+      </c>
+      <c r="P21" s="17">
+        <v>0.10486111111111111</v>
+      </c>
+      <c r="Q21" s="17">
+        <v>2.1527777777777778E-2</v>
+      </c>
+      <c r="R21" s="17">
+        <v>0.38124999999999998</v>
+      </c>
+      <c r="S21" s="1">
+        <v>1</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>3</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>19</v>
+      </c>
+      <c r="P22" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="17">
+        <v>3.4027777777777775E-2</v>
+      </c>
+      <c r="R22" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="S22" s="1">
+        <v>7</v>
+      </c>
+      <c r="T22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>2</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>4</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1</v>
+      </c>
+      <c r="N23" s="1">
+        <v>3</v>
+      </c>
+      <c r="O23" s="1">
+        <v>32</v>
+      </c>
+      <c r="P23" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="17">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="R23" s="17">
+        <v>0.77916666666666667</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0</v>
+      </c>
+      <c r="T23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>2</v>
+      </c>
+      <c r="M24" s="1">
+        <v>1</v>
+      </c>
+      <c r="N24" s="1">
+        <v>1</v>
+      </c>
+      <c r="O24" s="1">
+        <v>29</v>
+      </c>
+      <c r="P24" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="17">
+        <v>6.3194444444444442E-2</v>
+      </c>
+      <c r="R24" s="17">
+        <v>0.68194444444444446</v>
+      </c>
+      <c r="S24" s="1">
+        <v>0</v>
+      </c>
+      <c r="T24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>3</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <v>2</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1">
+        <v>2</v>
+      </c>
+      <c r="O25" s="1">
+        <v>32</v>
+      </c>
+      <c r="P25" s="17">
+        <v>8.4027777777777785E-2</v>
+      </c>
+      <c r="Q25" s="17">
+        <v>6.458333333333334E-2</v>
+      </c>
+      <c r="R25" s="17">
+        <v>0.7368055555555556</v>
+      </c>
+      <c r="S25" s="1">
+        <v>0</v>
+      </c>
+      <c r="T25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
+        <v>7</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <v>27</v>
+      </c>
+      <c r="P26" s="17">
+        <v>0.1423611111111111</v>
+      </c>
+      <c r="Q26" s="17">
+        <v>0</v>
+      </c>
+      <c r="R26" s="17">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="S26" s="1">
+        <v>15</v>
+      </c>
+      <c r="T26" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>4</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1">
+        <v>2</v>
+      </c>
+      <c r="O27" s="1">
+        <v>24</v>
+      </c>
+      <c r="P27" s="17">
+        <v>0.14305555555555555</v>
+      </c>
+      <c r="Q27" s="17">
+        <v>0</v>
+      </c>
+      <c r="R27" s="17">
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="S27" s="1">
+        <v>7</v>
+      </c>
+      <c r="T27" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1">
+        <v>3</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <v>2</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+      <c r="O28" s="1">
+        <v>27</v>
+      </c>
+      <c r="P28" s="17">
+        <v>8.1250000000000003E-2</v>
+      </c>
+      <c r="Q28" s="17">
+        <v>0</v>
+      </c>
+      <c r="R28" s="17">
+        <v>0.71736111111111112</v>
+      </c>
+      <c r="S28" s="1">
+        <v>0</v>
+      </c>
+      <c r="T28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <v>1</v>
+      </c>
+      <c r="O29" s="1">
+        <v>26</v>
+      </c>
+      <c r="P29" s="17">
+        <v>0.1361111111111111</v>
+      </c>
+      <c r="Q29" s="17">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="R29" s="17">
+        <v>0.68541666666666667</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0</v>
+      </c>
+      <c r="T29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>5</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <v>4</v>
+      </c>
+      <c r="M30" s="1">
+        <v>0</v>
+      </c>
+      <c r="N30" s="1">
+        <v>1</v>
+      </c>
+      <c r="O30" s="1">
+        <v>30</v>
+      </c>
+      <c r="P30" s="17">
+        <v>0.16597222222222222</v>
+      </c>
+      <c r="Q30" s="17">
+        <v>0</v>
+      </c>
+      <c r="R30" s="17">
+        <v>0.83680555555555558</v>
+      </c>
+      <c r="S30" s="1">
+        <v>0</v>
+      </c>
+      <c r="T30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <v>3</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1">
+        <v>6</v>
+      </c>
+      <c r="M31" s="1">
+        <v>0</v>
+      </c>
+      <c r="N31" s="1">
+        <v>1</v>
+      </c>
+      <c r="O31" s="1">
+        <v>14</v>
+      </c>
+      <c r="P31" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="17">
+        <v>0</v>
+      </c>
+      <c r="R31" s="17">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="S31" s="1">
+        <v>0</v>
+      </c>
+      <c r="T31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>2</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
+        <v>2</v>
+      </c>
+      <c r="M32" s="1">
+        <v>1</v>
+      </c>
+      <c r="N32" s="1">
+        <v>1</v>
+      </c>
+      <c r="O32" s="1">
+        <v>15</v>
+      </c>
+      <c r="P32" s="17">
+        <v>0.1076388888888889</v>
+      </c>
+      <c r="Q32" s="17">
+        <v>0</v>
+      </c>
+      <c r="R32" s="17">
+        <v>0.33402777777777776</v>
+      </c>
+      <c r="S32" s="1">
+        <v>0</v>
+      </c>
+      <c r="T32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>3</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1">
+        <v>1</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1">
+        <v>2</v>
+      </c>
+      <c r="O33" s="1">
+        <v>14</v>
+      </c>
+      <c r="P33" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="17">
+        <v>4.3749999999999997E-2</v>
+      </c>
+      <c r="R33" s="17">
+        <v>0.38611111111111113</v>
+      </c>
+      <c r="S33" s="1">
+        <v>3</v>
+      </c>
+      <c r="T33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G34" s="1">
+        <v>2</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <v>4</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
+        <v>9</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0</v>
+      </c>
+      <c r="O34" s="1">
+        <v>29</v>
+      </c>
+      <c r="P34" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="17">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="R34" s="17">
+        <v>0.68888888888888888</v>
+      </c>
+      <c r="S34" s="1">
+        <v>0</v>
+      </c>
+      <c r="T34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1">
+        <v>2</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1">
+        <v>6</v>
+      </c>
+      <c r="M35" s="1">
+        <v>1</v>
+      </c>
+      <c r="N35" s="1">
+        <v>1</v>
+      </c>
+      <c r="O35" s="1">
+        <v>26</v>
+      </c>
+      <c r="P35" s="17">
+        <v>0.1076388888888889</v>
+      </c>
+      <c r="Q35" s="17">
+        <v>0</v>
+      </c>
+      <c r="R35" s="17">
+        <v>0.69444444444444442</v>
+      </c>
+      <c r="S35" s="1">
+        <v>0</v>
+      </c>
+      <c r="T35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1">
+        <v>3</v>
+      </c>
+      <c r="M36" s="1">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+      <c r="O36" s="1">
+        <v>26</v>
+      </c>
+      <c r="P36" s="17">
+        <v>2.361111111111111E-2</v>
+      </c>
+      <c r="Q36" s="17">
+        <v>0</v>
+      </c>
+      <c r="R36" s="17">
+        <v>0.62013888888888891</v>
+      </c>
+      <c r="S36" s="1">
+        <v>0</v>
+      </c>
+      <c r="T36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1">
+        <v>5</v>
+      </c>
+      <c r="H37" s="1">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1">
+        <v>2</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0</v>
+      </c>
+      <c r="L37" s="1">
+        <v>3</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1">
+        <v>0</v>
+      </c>
+      <c r="O37" s="1">
+        <v>29</v>
+      </c>
+      <c r="P37" s="17">
+        <v>0.15347222222222223</v>
+      </c>
+      <c r="Q37" s="17">
+        <v>0</v>
+      </c>
+      <c r="R37" s="17">
+        <v>0.67222222222222228</v>
+      </c>
+      <c r="S37" s="1">
+        <v>1</v>
+      </c>
+      <c r="T37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U19">
+    <sortCondition ref="A2:A19"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="U1" location="'Scores (5-2-24)'!A1" display="HOME" xr:uid="{3C5641FA-C8B4-4C8D-82B2-9E6620D4B5B4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="L2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="18">
+        <v>2.4236111111111112</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M1" location="'Scores (4-29-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-2A00-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -95901,12 +98491,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -97650,8 +100240,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -97682,18 +100272,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O1" location="'Scores (4-29-24)'!A1" display="HOME"/>
+    <hyperlink ref="O1" location="'Scores (4-29-24)'!A1" display="HOME" xr:uid="{00000000-0004-0000-2D00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:J9"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -98030,16 +100620,16 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -98047,8 +100637,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E32D599-43B3-4A4B-9C16-AC5AECDFE8FA}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -98065,8 +100655,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35784E2-AC8B-458A-863A-007FC5E470EB}">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -98095,14 +100685,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O1" location="'Scores (4-29-24)'!A1" display="HOME"/>
+    <hyperlink ref="O1" location="'Scores (4-29-24)'!A1" display="HOME" xr:uid="{3C1FFAA5-D1F4-4DCD-8BFB-BC44970DD99F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -98220,21 +100810,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A7" location="'Offense (4-21-24)'!A1" display="Offense"/>
-    <hyperlink ref="A8" location="'Goalies (4-21-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="A7" location="'Offense (4-21-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="A8" location="'Goalies (4-21-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -98247,7 +100837,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -98365,21 +100955,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A7" location="'Offense (4-22-24)'!A1" display="Offense"/>
-    <hyperlink ref="A8" location="'Goalies (4-22-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="A7" location="'Offense (4-22-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="A8" location="'Goalies (4-22-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -98392,7 +100982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -98513,21 +101103,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E6" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A7" location="'Offense (4-23-24)'!A1" display="Offense"/>
-    <hyperlink ref="A8" location="'Goalies (4-23-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="A7" location="'Offense (4-23-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="A8" location="'Goalies (4-23-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -98540,7 +101130,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -98647,21 +101237,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E5" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A6" location="'Offense (4-24-24)'!A1" display="Offense"/>
-    <hyperlink ref="A7" location="'Goalies (4-24-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="A6" location="'Offense (4-24-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="A7" location="'Goalies (4-24-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>
@@ -98674,7 +101264,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -98764,21 +101354,21 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>$AA$1:$AA$2</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E1" location="Index!A1" display="INDEX"/>
-    <hyperlink ref="A5" location="'Offense (4-25-24)'!A1" display="Offense"/>
-    <hyperlink ref="A6" location="'Goalies (4-25-24)'!A1" display="Goalies"/>
+    <hyperlink ref="E1" location="Index!A1" display="INDEX" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="A5" location="'Offense (4-25-24)'!A1" display="Offense" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="A6" location="'Goalies (4-25-24)'!A1" display="Goalies" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000001000000}">
           <x14:formula1>
             <xm:f>Teams!$C$2:$C$17</xm:f>
           </x14:formula1>

</xml_diff>